<commit_message>
CYRS Updated according to CYRS Review Document Signed-off-by: ahmed.zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_CYRS_Review.xlsx
+++ b/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_CYRS_Review.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B47FFBC-5671-4DBB-A494-759A46C31AFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -161,12 +162,15 @@
   </si>
   <si>
     <t xml:space="preserve">I found to documents for the CYRS v1.0 and v1.1 , while we should update only in one document , not every change we will make new document </t>
+  </si>
+  <si>
+    <t>The refer is applied using CTRL + Click</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -531,12 +535,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,40 +584,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -923,10 +927,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -937,96 +941,96 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="38"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="24">
+      <c r="C7" s="26"/>
+      <c r="D7" s="31">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="33" t="s">
@@ -1060,83 +1064,66 @@
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24" t="s">
+      <c r="D13" s="31"/>
+      <c r="E13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="25"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1153,6 +1140,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1160,11 +1164,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1230,7 +1234,7 @@
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I2" s="10"/>
     </row>
@@ -1255,14 +1259,14 @@
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I3" s="10"/>
       <c r="K3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>35</v>
       </c>
@@ -1285,7 +1289,9 @@
       <c r="H4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="K4" t="s">
         <v>21</v>
       </c>
@@ -1339,7 +1345,7 @@
         <v>19</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="K6" s="40" t="s">
+      <c r="K6" s="24" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1875,10 +1881,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$K$3:$K$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$K$6:$K$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated Decision status Signed-off-by: Ahmed-Zoher <59732468+Ahmed-Zoher@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_CYRS_Review.xlsx
+++ b/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_CYRS_Review.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B47FFBC-5671-4DBB-A494-759A46C31AFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA804C4E-5857-4880-946E-16E2B12D36D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -536,12 +536,42 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -553,36 +583,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -941,189 +941,206 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="29"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="30"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="30"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="31" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="31">
+      <c r="C7" s="33"/>
+      <c r="D7" s="25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="31" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="31" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="35"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="s">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="32"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1140,23 +1157,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1168,7 +1168,7 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,7 +1232,9 @@
       <c r="F2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>22</v>
       </c>
@@ -1257,7 +1259,9 @@
       <c r="F3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>22</v>
       </c>
@@ -1285,7 +1289,9 @@
       <c r="F4" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H4" s="10" t="s">
         <v>19</v>
       </c>
@@ -1315,7 +1321,9 @@
       <c r="F5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="10" t="s">
         <v>19</v>
       </c>
@@ -1340,7 +1348,9 @@
       <c r="F6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>19</v>
       </c>
@@ -1368,7 +1378,9 @@
       <c r="F7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="10" t="s">
         <v>19</v>
       </c>
@@ -1396,7 +1408,9 @@
       <c r="F8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H8" s="10" t="s">
         <v>19</v>
       </c>
@@ -1421,7 +1435,9 @@
       <c r="F9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H9" s="10" t="s">
         <v>19</v>
       </c>
@@ -1446,7 +1462,9 @@
       <c r="F10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H10" s="10" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Update the review sheet for CYRS , HSI
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_CYRS_Review.xlsx
+++ b/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_CYRS_Review.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA804C4E-5857-4880-946E-16E2B12D36D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -165,12 +164,18 @@
   </si>
   <si>
     <t>The refer is applied using CTRL + Click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update the status of each point </t>
+  </si>
+  <si>
+    <t>PO4_DGELV_DIGITAL ELEVATOR_CYRS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -470,7 +475,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -536,12 +541,42 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,40 +591,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -708,7 +716,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -743,7 +751,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -927,11 +935,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -941,96 +949,96 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="39"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="40"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="40"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="25">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="31">
+        <v>1.4</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="33">
+        <v>44076</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="34" t="s">
@@ -1064,83 +1072,74 @@
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25" t="s">
+      <c r="D13" s="31"/>
+      <c r="E13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="26"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
+      <c r="B14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="33">
+        <v>44076</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1157,6 +1156,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1164,11 +1180,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1293,7 +1309,7 @@
         <v>20</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>47</v>
@@ -1325,7 +1341,7 @@
         <v>20</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I5" s="12"/>
     </row>
@@ -1352,7 +1368,7 @@
         <v>20</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I6" s="12"/>
       <c r="K6" s="24" t="s">
@@ -1382,7 +1398,7 @@
         <v>20</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I7" s="12"/>
       <c r="K7" t="s">
@@ -1412,7 +1428,7 @@
         <v>20</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I8" s="12"/>
     </row>
@@ -1439,7 +1455,7 @@
         <v>20</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I9" s="12"/>
     </row>
@@ -1466,7 +1482,7 @@
         <v>20</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I10" s="12"/>
       <c r="K10" t="s">
@@ -1899,10 +1915,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
       <formula1>$K$3:$K$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
       <formula1>$K$6:$K$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>